<commit_message>
fix some spacing issues, add number padding
</commit_message>
<xml_diff>
--- a/cis_win2022_from_audit.xlsx
+++ b/cis_win2022_from_audit.xlsx
@@ -526,7 +526,8 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -566,7 +567,8 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -604,7 +606,8 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -644,7 +647,8 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -694,7 +698,8 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -742,7 +747,8 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -780,7 +786,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53|SC-28, 800-53|SC-28(1), 800-53r5|IA-5(1), 800-53r5|SC-28, 800-53r5|SC-28(1)</t>
+          <t>800-53|IA-5(1)
+800-53|SC-28
+800-53|SC-28(1)
+800-53r5|IA-5(1)
+800-53r5|SC-28
+800-53r5|SC-28(1)</t>
         </is>
       </c>
     </row>
@@ -819,7 +830,10 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -859,7 +873,10 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -907,7 +924,10 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -946,7 +966,10 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -987,7 +1010,14 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1062,14 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1085,7 +1122,14 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1182,14 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1227,14 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1276,14 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1321,14 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1366,14 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1333,7 +1412,14 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1374,7 +1460,14 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1514,14 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1559,14 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1604,14 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1649,14 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1582,7 +1703,14 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1620,7 +1748,14 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1801,14 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1714,7 +1856,14 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1906,14 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1978,14 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1877,7 +2040,14 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1931,7 +2101,14 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -1979,7 +2156,14 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2029,7 +2213,14 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2261,14 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2112,7 +2310,14 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2364,14 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2409,8 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>800-53|AC-2(1), 800-53r5|AC-2(1)</t>
+          <t>800-53|AC-2(1)
+800-53r5|AC-2(1)</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2451,10 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2492,8 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>800-53|IA-5c., 800-53r5|IA-5c.</t>
+          <t>800-53|IA-5c.
+800-53r5|IA-5c.</t>
         </is>
       </c>
     </row>
@@ -2314,7 +2531,8 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -2352,7 +2570,8 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -2414,7 +2633,8 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2672,8 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>800-53|SI-4, 800-53r5|SI-4</t>
+          <t>800-53|SI-4
+800-53r5|SI-4</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2711,8 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -2528,7 +2750,14 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -2567,7 +2796,10 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2606,7 +2838,8 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>800-53|AU-2, 800-53r5|AU-2</t>
+          <t>800-53|AU-2
+800-53r5|AU-2</t>
         </is>
       </c>
     </row>
@@ -2645,7 +2878,14 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>800-53|CM-7(2), 800-53|CM-8(3), 800-53|CM-10, 800-53|CM-11, 800-53r5|CM-7(2), 800-53r5|CM-8(3), 800-53r5|CM-10, 800-53r5|CM-11</t>
+          <t>800-53|CM-7(2)
+800-53|CM-8(3)
+800-53|CM-10
+800-53|CM-11
+800-53r5|CM-7(2)
+800-53r5|CM-8(3)
+800-53r5|CM-10
+800-53r5|CM-11</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2923,10 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2964,10 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2759,7 +3005,10 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2797,7 +3046,10 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -2841,7 +3093,8 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -2884,7 +3137,8 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -2928,7 +3182,8 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -2971,7 +3226,8 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -3015,7 +3271,8 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -3058,7 +3315,8 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -3102,7 +3360,8 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3404,8 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3444,8 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -3222,7 +3483,10 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -3260,7 +3524,10 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -3300,7 +3567,8 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>800-53|AC-2(1), 800-53r5|AC-2(1)</t>
+          <t>800-53|AC-2(1)
+800-53r5|AC-2(1)</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3606,8 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3646,8 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3685,8 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>800-53|SI-4, 800-53r5|SI-4</t>
+          <t>800-53|SI-4
+800-53r5|SI-4</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3724,8 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>800-53|SI-4, 800-53r5|SI-4</t>
+          <t>800-53|SI-4
+800-53r5|SI-4</t>
         </is>
       </c>
     </row>
@@ -3491,7 +3763,10 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>800-53|MP-7, 800-53|SI-3, 800-53r5|MP-7, 800-53r5|SI-3</t>
+          <t>800-53|MP-7
+800-53|SI-3
+800-53r5|MP-7
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3529,7 +3804,10 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>800-53|MP-7, 800-53|SI-3, 800-53r5|MP-7, 800-53r5|SI-3</t>
+          <t>800-53|MP-7
+800-53|SI-3
+800-53r5|MP-7
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3567,7 +3845,8 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3607,7 +3886,8 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3651,7 +3931,8 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -3689,7 +3970,10 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -3727,7 +4011,8 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -3921,7 +4206,12 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>800-53|SC-7(3), 800-53|SC-7(4), 800-53|SI-16, 800-53r5|SC-7(3), 800-53r5|SC-7(4), 800-53r5|SI-16</t>
+          <t>800-53|SC-7(3)
+800-53|SC-7(4)
+800-53|SI-16
+800-53r5|SC-7(3)
+800-53r5|SC-7(4)
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -3963,7 +4253,8 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4308,10 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -4055,7 +4349,8 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>800-53|AC-2(1), 800-53r5|AC-2(1)</t>
+          <t>800-53|AC-2(1)
+800-53r5|AC-2(1)</t>
         </is>
       </c>
     </row>
@@ -4094,7 +4389,10 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -4135,7 +4433,10 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>800-53|AU-11, 800-53|SI-12, 800-53r5|AU-11, 800-53r5|SI-12</t>
+          <t>800-53|AU-11
+800-53|SI-12
+800-53r5|AU-11
+800-53r5|SI-12</t>
         </is>
       </c>
     </row>
@@ -4174,7 +4475,10 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>800-53|AU-11, 800-53|SI-12, 800-53r5|AU-11, 800-53r5|SI-12</t>
+          <t>800-53|AU-11
+800-53|SI-12
+800-53r5|AU-11
+800-53r5|SI-12</t>
         </is>
       </c>
     </row>
@@ -4214,7 +4518,10 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -4255,7 +4562,10 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>800-53|AC-17(6), 800-53|IA-2, 800-53r5|AC-17(6), 800-53r5|IA-2</t>
+          <t>800-53|AC-17(6)
+800-53|IA-2
+800-53r5|AC-17(6)
+800-53r5|IA-2</t>
         </is>
       </c>
     </row>
@@ -4294,7 +4604,8 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>800-53|SC-7(8), 800-53r5|SC-7(8)</t>
+          <t>800-53|SC-7(8)
+800-53r5|SC-7(8)</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4650,16 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -4381,7 +4701,16 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4748,16 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -4460,7 +4798,12 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>800-53|CM-10, 800-53|CM-11, 800-53|SC-18, 800-53r5|CM-10, 800-53r5|CM-11, 800-53r5|SC-18</t>
+          <t>800-53|CM-10
+800-53|CM-11
+800-53|SC-18
+800-53r5|CM-10
+800-53r5|CM-11
+800-53r5|SC-18</t>
         </is>
       </c>
     </row>
@@ -4498,7 +4841,10 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4882,8 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>800-53|MP-7, 800-53r5|MP-7</t>
+          <t>800-53|MP-7
+800-53r5|MP-7</t>
         </is>
       </c>
     </row>
@@ -4574,7 +4921,8 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>800-53|MP-7, 800-53r5|MP-7</t>
+          <t>800-53|MP-7
+800-53r5|MP-7</t>
         </is>
       </c>
     </row>
@@ -4613,7 +4961,8 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>800-53|MP-7, 800-53r5|MP-7</t>
+          <t>800-53|MP-7
+800-53r5|MP-7</t>
         </is>
       </c>
     </row>
@@ -4675,7 +5024,8 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -4716,7 +5066,8 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -4756,7 +5107,8 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>800-53|AC-2(9), 800-53r5|AC-2(9)</t>
+          <t>800-53|AC-2(9)
+800-53r5|AC-2(9)</t>
         </is>
       </c>
     </row>
@@ -4799,7 +5151,8 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -4837,7 +5190,10 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -4878,7 +5234,8 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>800-53|AC-11, 800-53r5|AC-11</t>
+          <t>800-53|AC-11
+800-53r5|AC-11</t>
         </is>
       </c>
     </row>
@@ -4916,7 +5273,16 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -4954,7 +5320,16 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -4992,7 +5367,16 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -5030,7 +5414,16 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -5068,7 +5461,16 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -5108,7 +5510,8 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>800-53|SC-7(21), 800-53r5|SC-7(21)</t>
+          <t>800-53|SC-7(21)
+800-53r5|SC-7(21)</t>
         </is>
       </c>
     </row>
@@ -5146,7 +5549,8 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -5188,7 +5592,13 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>800-53|RA-5, 800-53|SI-2, 800-53|SI-2(2), 800-53r5|RA-5, 800-53r5|RA-7, 800-53r5|SI-2, 800-53r5|SI-2(2)</t>
+          <t>800-53|RA-5
+800-53|SI-2
+800-53|SI-2(2)
+800-53r5|RA-5
+800-53r5|RA-7
+800-53r5|SI-2
+800-53r5|SI-2(2)</t>
         </is>
       </c>
     </row>
@@ -5239,7 +5649,13 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>800-53|RA-5, 800-53|SI-2, 800-53|SI-2(2), 800-53r5|RA-5, 800-53r5|RA-7, 800-53r5|SI-2, 800-53r5|SI-2(2)</t>
+          <t>800-53|RA-5
+800-53|SI-2
+800-53|SI-2(2)
+800-53r5|RA-5
+800-53r5|RA-7
+800-53r5|SI-2
+800-53r5|SI-2(2)</t>
         </is>
       </c>
     </row>
@@ -5278,7 +5694,13 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>800-53|RA-5, 800-53|SI-2, 800-53|SI-2(2), 800-53r5|RA-5, 800-53r5|RA-7, 800-53r5|SI-2, 800-53r5|SI-2(2)</t>
+          <t>800-53|RA-5
+800-53|SI-2
+800-53|SI-2(2)
+800-53r5|RA-5
+800-53r5|RA-7
+800-53r5|SI-2
+800-53r5|SI-2(2)</t>
         </is>
       </c>
     </row>
@@ -5321,7 +5743,10 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>800-53|CM-7(5), 800-53|CM-10, 800-53r5|CM-7(5), 800-53r5|CM-10</t>
+          <t>800-53|CM-7(5)
+800-53|CM-10
+800-53r5|CM-7(5)
+800-53r5|CM-10</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5832,8 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -5445,7 +5871,8 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -5488,7 +5915,23 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -5536,7 +5979,8 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>800-53|AC-2(9), 800-53r5|AC-2(9)</t>
+          <t>800-53|AC-2(9)
+800-53r5|AC-2(9)</t>
         </is>
       </c>
     </row>
@@ -5578,7 +6022,8 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -5626,7 +6071,10 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -5671,7 +6119,10 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -5717,7 +6168,8 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>800-53|SC-8, 800-53r5|SC-8</t>
+          <t>800-53|SC-8
+800-53r5|SC-8</t>
         </is>
       </c>
     </row>
@@ -5759,7 +6211,8 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -5809,7 +6262,23 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -5855,7 +6324,12 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53|SC-28, 800-53|SC-28(1), 800-53r5|IA-5(1), 800-53r5|SC-28, 800-53r5|SC-28(1)</t>
+          <t>800-53|IA-5(1)
+800-53|SC-28
+800-53|SC-28(1)
+800-53r5|IA-5(1)
+800-53r5|SC-28
+800-53r5|SC-28(1)</t>
         </is>
       </c>
     </row>
@@ -5919,7 +6393,8 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -5958,7 +6433,8 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53r5|CM-6</t>
+          <t>800-53|CM-6
+800-53r5|CM-6</t>
         </is>
       </c>
     </row>
@@ -5997,7 +6473,8 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>800-53|SC-7(12), 800-53r5|SC-7(12)</t>
+          <t>800-53|SC-7(12)
+800-53r5|SC-7(12)</t>
         </is>
       </c>
     </row>
@@ -6036,7 +6513,23 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6570,8 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53r5|CM-6</t>
+          <t>800-53|CM-6
+800-53r5|CM-6</t>
         </is>
       </c>
     </row>
@@ -6122,7 +6616,8 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -6161,7 +6656,14 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>800-53|AC-2(5), 800-53|AC-11, 800-53|AC-11(1), 800-53|AC-12, 800-53r5|AC-2(5), 800-53r5|AC-11, 800-53r5|AC-11(1), 800-53r5|AC-12</t>
+          <t>800-53|AC-2(5)
+800-53|AC-11
+800-53|AC-11(1)
+800-53|AC-12
+800-53r5|AC-2(5)
+800-53r5|AC-11
+800-53r5|AC-11(1)
+800-53r5|AC-12</t>
         </is>
       </c>
     </row>
@@ -6200,7 +6702,22 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>800-53|AC-18, 800-53|AC-18(1), 800-53|AC-18(3), 800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53r5|AC-18, 800-53r5|AC-18(1), 800-53r5|AC-18(3), 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9</t>
+          <t>800-53|AC-18
+800-53|AC-18(1)
+800-53|AC-18(3)
+800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53r5|AC-18
+800-53r5|AC-18(1)
+800-53r5|AC-18(3)
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9</t>
         </is>
       </c>
     </row>
@@ -6238,7 +6755,10 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -6276,7 +6796,8 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -6342,7 +6863,23 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -6384,7 +6921,16 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -6422,7 +6968,10 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -6461,7 +7010,10 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -6500,7 +7052,8 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -6546,7 +7099,8 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>800-53|AC-6(8), 800-53r5|AC-6(8)</t>
+          <t>800-53|AC-6(8)
+800-53r5|AC-6(8)</t>
         </is>
       </c>
     </row>
@@ -6592,7 +7146,8 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -6630,7 +7185,8 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -6668,7 +7224,8 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -6706,7 +7263,8 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -6744,7 +7302,8 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -6782,7 +7341,8 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>800-53|IA-3(1), 800-53r5|IA-3(1)</t>
+          <t>800-53|IA-3(1)
+800-53r5|IA-3(1)</t>
         </is>
       </c>
     </row>
@@ -6820,7 +7380,8 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -6865,7 +7426,8 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>800-53|SI-4, 800-53r5|SI-4</t>
+          <t>800-53|SI-4
+800-53r5|SI-4</t>
         </is>
       </c>
     </row>
@@ -6905,7 +7467,8 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -6949,7 +7512,8 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -6988,7 +7552,23 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7027,7 +7607,23 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7066,7 +7662,23 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7105,7 +7717,23 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7143,7 +7771,10 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -7181,7 +7812,23 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7220,7 +7867,10 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>800-53|CM-7(5), 800-53|CM-10, 800-53r5|CM-7(5), 800-53r5|CM-10</t>
+          <t>800-53|CM-7(5)
+800-53|CM-10
+800-53r5|CM-7(5)
+800-53r5|CM-10</t>
         </is>
       </c>
     </row>
@@ -7258,7 +7908,10 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -7302,7 +7955,8 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>800-53|CM-8, 800-53r5|CM-8</t>
+          <t>800-53|CM-8
+800-53r5|CM-8</t>
         </is>
       </c>
     </row>
@@ -7344,7 +7998,8 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>800-53|CP-9, 800-53r5|CP-9</t>
+          <t>800-53|CP-9
+800-53r5|CP-9</t>
         </is>
       </c>
     </row>
@@ -7386,7 +8041,8 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1)(d), 800-53r5|IA-5(1)(d)</t>
+          <t>800-53|IA-5(1)(d)
+800-53r5|IA-5(1)(d)</t>
         </is>
       </c>
     </row>
@@ -7429,7 +8085,16 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -7470,7 +8135,8 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -7511,7 +8177,8 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -7552,7 +8219,8 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -7593,7 +8261,8 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -7638,7 +8307,8 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -7675,7 +8345,8 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -7713,7 +8384,23 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -7751,7 +8438,8 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -7789,7 +8477,8 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -7827,7 +8516,8 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -7865,7 +8555,10 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -7904,7 +8597,10 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -7946,7 +8642,10 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -7990,7 +8689,8 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>800-53|AU-2, 800-53r5|AU-2</t>
+          <t>800-53|AU-2
+800-53r5|AU-2</t>
         </is>
       </c>
     </row>
@@ -8028,7 +8728,8 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>800-53|AC-11, 800-53r5|AC-11</t>
+          <t>800-53|AC-11
+800-53r5|AC-11</t>
         </is>
       </c>
     </row>
@@ -8066,7 +8767,8 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>800-53|AC-11, 800-53r5|AC-11</t>
+          <t>800-53|AC-11
+800-53r5|AC-11</t>
         </is>
       </c>
     </row>
@@ -8105,7 +8807,10 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -8143,7 +8848,10 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -8188,7 +8896,8 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -8228,7 +8937,8 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>800-53|SI-16, 800-53r5|SI-16</t>
+          <t>800-53|SI-16
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -8275,7 +8985,8 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>800-53|IA-5, 800-53r5|IA-5</t>
+          <t>800-53|IA-5
+800-53r5|IA-5</t>
         </is>
       </c>
     </row>
@@ -8314,7 +9025,10 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>800-53|AU-7, 800-53|AU-8, 800-53r5|AU-7, 800-53r5|AU-8</t>
+          <t>800-53|AU-7
+800-53|AU-8
+800-53r5|AU-7
+800-53r5|AU-8</t>
         </is>
       </c>
     </row>
@@ -8355,7 +9069,10 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>800-53|AU-7, 800-53|AU-8, 800-53r5|AU-7, 800-53r5|AU-8</t>
+          <t>800-53|AU-7
+800-53|AU-8
+800-53r5|AU-7
+800-53r5|AU-8</t>
         </is>
       </c>
     </row>
@@ -8394,7 +9111,12 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>800-53|CM-7(5), 800-53|CM-10, 800-53|SI-16, 800-53r5|CM-7(5), 800-53r5|CM-10, 800-53r5|SI-16</t>
+          <t>800-53|CM-7(5)
+800-53|CM-10
+800-53|SI-16
+800-53r5|CM-7(5)
+800-53r5|CM-10
+800-53r5|SI-16</t>
         </is>
       </c>
     </row>
@@ -8432,7 +9154,10 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -8470,7 +9195,8 @@
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>800-53|AC-3, 800-53r5|AC-3</t>
+          <t>800-53|AC-3
+800-53r5|AC-3</t>
         </is>
       </c>
     </row>
@@ -8510,7 +9236,8 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>800-53|AC-2(9), 800-53r5|AC-2(9)</t>
+          <t>800-53|AC-2(9)
+800-53r5|AC-2(9)</t>
         </is>
       </c>
     </row>
@@ -8551,7 +9278,8 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -8590,7 +9318,8 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>800-53|SI-3, 800-53r5|SI-3</t>
+          <t>800-53|SI-3
+800-53r5|SI-3</t>
         </is>
       </c>
     </row>
@@ -8631,7 +9360,8 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>800-53|AC-11, 800-53r5|AC-11</t>
+          <t>800-53|AC-11
+800-53r5|AC-11</t>
         </is>
       </c>
     </row>
@@ -8669,7 +9399,8 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>800-53|CM-7b., 800-53r5|CM-7b.</t>
+          <t>800-53|CM-7b.
+800-53r5|CM-7b.</t>
         </is>
       </c>
     </row>
@@ -8707,7 +9438,10 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>800-53|CM-6, 800-53|CM-7, 800-53r5|CM-6, 800-53r5|CM-7</t>
+          <t>800-53|CM-6
+800-53|CM-7
+800-53r5|CM-6
+800-53r5|CM-7</t>
         </is>
       </c>
     </row>
@@ -8744,7 +9478,18 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8789,7 +9534,18 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8827,7 +9583,18 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8871,7 +9638,18 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8908,7 +9686,18 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8945,7 +9734,18 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -8984,7 +9784,18 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9025,7 +9836,18 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9062,7 +9884,18 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9102,7 +9935,18 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9142,7 +9986,18 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9184,7 +10039,18 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9225,7 +10091,18 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9263,7 +10140,18 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9301,7 +10189,18 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9343,7 +10242,18 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9381,7 +10291,18 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9418,7 +10339,18 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9455,7 +10387,18 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9505,7 +10448,18 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9560,7 +10514,18 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9597,7 +10562,18 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9635,7 +10611,18 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9673,7 +10660,18 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9712,7 +10710,18 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9750,7 +10759,18 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9787,7 +10807,18 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9825,7 +10856,18 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9863,7 +10905,18 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9900,7 +10953,18 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9937,7 +11001,18 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -9985,7 +11060,18 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10024,7 +11110,18 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10062,7 +11159,18 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10100,7 +11208,18 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10143,7 +11262,18 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10181,7 +11311,18 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -10218,7 +11359,10 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53|IA-2(2), 800-53r5|AC-6(10), 800-53r5|IA-2(2)</t>
+          <t>800-53|AC-6(10)
+800-53|IA-2(2)
+800-53r5|AC-6(10)
+800-53r5|IA-2(2)</t>
         </is>
       </c>
     </row>
@@ -10267,7 +11411,8 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -10309,7 +11454,8 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>800-53|AC-6(3), 800-53r5|AC-6(3)</t>
+          <t>800-53|AC-6(3)
+800-53r5|AC-6(3)</t>
         </is>
       </c>
     </row>
@@ -10346,7 +11492,8 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>800-53|AC-3, 800-53r5|AC-3</t>
+          <t>800-53|AC-3
+800-53r5|AC-3</t>
         </is>
       </c>
     </row>
@@ -10384,7 +11531,8 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -10422,7 +11570,8 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -10460,7 +11609,8 @@
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -10497,7 +11647,8 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -10545,7 +11696,8 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>800-53|IA-2(2), 800-53r5|IA-2(2)</t>
+          <t>800-53|IA-2(2)
+800-53r5|IA-2(2)</t>
         </is>
       </c>
     </row>
@@ -10588,7 +11740,8 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>800-53|AC-6(7)(b), 800-53r5|AC-6(7)(b)</t>
+          <t>800-53|AC-6(7)(b)
+800-53r5|AC-6(7)(b)</t>
         </is>
       </c>
     </row>
@@ -10706,7 +11859,8 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>800-53|AC-6(7)(b), 800-53r5|AC-6(7)(b)</t>
+          <t>800-53|AC-6(7)(b)
+800-53r5|AC-6(7)(b)</t>
         </is>
       </c>
     </row>
@@ -10788,7 +11942,8 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>800-53|AC-6(7)(b), 800-53r5|AC-6(7)(b)</t>
+          <t>800-53|AC-6(7)(b)
+800-53r5|AC-6(7)(b)</t>
         </is>
       </c>
     </row>
@@ -10858,7 +12013,8 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>800-53|AC-6(7)(b), 800-53r5|AC-6(7)(b)</t>
+          <t>800-53|AC-6(7)(b)
+800-53r5|AC-6(7)(b)</t>
         </is>
       </c>
     </row>
@@ -10928,7 +12084,8 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>800-53|AC-6(7)(b), 800-53r5|AC-6(7)(b)</t>
+          <t>800-53|AC-6(7)(b)
+800-53r5|AC-6(7)(b)</t>
         </is>
       </c>
     </row>
@@ -10965,7 +12122,8 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>800-53|AC-2(1), 800-53r5|AC-2(1)</t>
+          <t>800-53|AC-2(1)
+800-53r5|AC-2(1)</t>
         </is>
       </c>
     </row>
@@ -11002,7 +12160,8 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>800-53|IA-3, 800-53r5|IA-3</t>
+          <t>800-53|IA-3
+800-53r5|IA-3</t>
         </is>
       </c>
     </row>
@@ -11042,7 +12201,16 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -11080,7 +12248,14 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -11119,7 +12294,14 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -11156,7 +12338,8 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -11197,7 +12380,23 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -11240,7 +12439,16 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -11278,7 +12486,12 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53|SC-28, 800-53|SC-28(1), 800-53r5|IA-5(1), 800-53r5|SC-28, 800-53r5|SC-28(1)</t>
+          <t>800-53|IA-5(1)
+800-53|SC-28
+800-53|SC-28(1)
+800-53r5|IA-5(1)
+800-53r5|SC-28
+800-53r5|SC-28(1)</t>
         </is>
       </c>
     </row>
@@ -11317,7 +12530,8 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>800-53|AC-2(12), 800-53r5|AC-2(12)</t>
+          <t>800-53|AC-2(12)
+800-53r5|AC-2(12)</t>
         </is>
       </c>
     </row>
@@ -11361,7 +12575,16 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -11401,7 +12624,16 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -11441,7 +12673,16 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -11479,7 +12720,8 @@
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>800-53|IA-5, 800-53r5|IA-5</t>
+          <t>800-53|IA-5
+800-53r5|IA-5</t>
         </is>
       </c>
     </row>
@@ -11516,7 +12758,8 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -11554,7 +12797,8 @@
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -11591,7 +12835,8 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>800-53|IA-5, 800-53r5|IA-5</t>
+          <t>800-53|IA-5
+800-53r5|IA-5</t>
         </is>
       </c>
     </row>
@@ -11627,7 +12872,8 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>800-53|IA-5, 800-53r5|IA-5</t>
+          <t>800-53|IA-5
+800-53r5|IA-5</t>
         </is>
       </c>
     </row>
@@ -11664,7 +12910,8 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>800-53|CM-6b., 800-53r5|CM-6b.</t>
+          <t>800-53|CM-6b.
+800-53r5|CM-6b.</t>
         </is>
       </c>
     </row>
@@ -11701,7 +12948,23 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -11741,7 +13004,8 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>800-53|AC-2(9), 800-53r5|AC-2(9)</t>
+          <t>800-53|AC-2(9)
+800-53r5|AC-2(9)</t>
         </is>
       </c>
     </row>
@@ -11778,7 +13042,8 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>800-53|AC-6(1), 800-53r5|AC-6(1)</t>
+          <t>800-53|AC-6(1)
+800-53r5|AC-6(1)</t>
         </is>
       </c>
     </row>
@@ -11820,7 +13085,8 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>800-53|AC-6(10), 800-53r5|AC-6(10)</t>
+          <t>800-53|AC-6(10)
+800-53r5|AC-6(10)</t>
         </is>
       </c>
     </row>
@@ -11857,7 +13123,8 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>800-53|AC-6(8), 800-53r5|AC-6(8)</t>
+          <t>800-53|AC-6(8)
+800-53r5|AC-6(8)</t>
         </is>
       </c>
     </row>
@@ -11903,7 +13170,8 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>800-53|AC-6(8), 800-53r5|AC-6(8)</t>
+          <t>800-53|AC-6(8)
+800-53r5|AC-6(8)</t>
         </is>
       </c>
     </row>
@@ -11941,7 +13209,8 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>800-53|AC-6(1), 800-53r5|AC-6(1)</t>
+          <t>800-53|AC-6(1)
+800-53r5|AC-6(1)</t>
         </is>
       </c>
     </row>
@@ -11978,7 +13247,8 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>800-53|AC-6(1), 800-53r5|AC-6(1)</t>
+          <t>800-53|AC-6(1)
+800-53r5|AC-6(1)</t>
         </is>
       </c>
     </row>
@@ -12019,7 +13289,8 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>800-53|SC-29(1), 800-53r5|SC-29(1)</t>
+          <t>800-53|SC-29(1)
+800-53r5|SC-29(1)</t>
         </is>
       </c>
     </row>
@@ -12058,7 +13329,14 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12</t>
         </is>
       </c>
     </row>
@@ -12096,7 +13374,8 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>800-53|AU-4, 800-53r5|AU-4</t>
+          <t>800-53|AU-4
+800-53r5|AU-4</t>
         </is>
       </c>
     </row>
@@ -12134,7 +13413,18 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>800-53|AC-2, 800-53|AC-3, 800-53|AC-6, 800-53|AC-6(1), 800-53|AC-6(7), 800-53|AU-9(4), 800-53r5|AC-2, 800-53r5|AC-5, 800-53r5|AC-6, 800-53r5|AC-6(1), 800-53r5|AC-6(7), 800-53r5|AU-9(4)</t>
+          <t>800-53|AC-2
+800-53|AC-3
+800-53|AC-6
+800-53|AC-6(1)
+800-53|AC-6(7)
+800-53|AU-9(4)
+800-53r5|AC-2
+800-53r5|AC-5
+800-53r5|AC-6
+800-53r5|AC-6(1)
+800-53r5|AC-6(7)
+800-53r5|AU-9(4)</t>
         </is>
       </c>
     </row>
@@ -12176,7 +13466,16 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12214,7 +13513,16 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12252,7 +13560,16 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12290,7 +13607,8 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>800-53|AC-2(1), 800-53r5|AC-2(1)</t>
+          <t>800-53|AC-2(1)
+800-53r5|AC-2(1)</t>
         </is>
       </c>
     </row>
@@ -12329,7 +13647,8 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -12367,7 +13686,16 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12405,7 +13733,10 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -12445,7 +13776,10 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>800-53|AC-7, 800-53|AC-19, 800-53r5|AC-7, 800-53r5|AC-19</t>
+          <t>800-53|AC-7
+800-53|AC-19
+800-53r5|AC-7
+800-53r5|AC-19</t>
         </is>
       </c>
     </row>
@@ -12483,7 +13817,14 @@
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>800-53|AC-2(5), 800-53|AC-11, 800-53|AC-11(1), 800-53|AC-12, 800-53r5|AC-2(5), 800-53r5|AC-11, 800-53r5|AC-11(1), 800-53r5|AC-12</t>
+          <t>800-53|AC-2(5)
+800-53|AC-11
+800-53|AC-11(1)
+800-53|AC-12
+800-53r5|AC-2(5)
+800-53r5|AC-11
+800-53r5|AC-11(1)
+800-53r5|AC-12</t>
         </is>
       </c>
     </row>
@@ -12521,7 +13862,8 @@
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>800-53|AC-8, 800-53r5|AC-8</t>
+          <t>800-53|AC-8
+800-53r5|AC-8</t>
         </is>
       </c>
     </row>
@@ -12557,7 +13899,8 @@
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>800-53|AC-8, 800-53r5|AC-8</t>
+          <t>800-53|AC-8
+800-53r5|AC-8</t>
         </is>
       </c>
     </row>
@@ -12594,7 +13937,8 @@
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>800-53|IA-5(1), 800-53r5|IA-5(1)</t>
+          <t>800-53|IA-5(1)
+800-53r5|IA-5(1)</t>
         </is>
       </c>
     </row>
@@ -12631,7 +13975,14 @@
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>800-53|AC-2(5), 800-53|AC-11, 800-53|AC-11(1), 800-53|AC-12, 800-53r5|AC-2(5), 800-53r5|AC-11, 800-53r5|AC-11(1), 800-53r5|AC-12</t>
+          <t>800-53|AC-2(5)
+800-53|AC-11
+800-53|AC-11(1)
+800-53|AC-12
+800-53r5|AC-2(5)
+800-53r5|AC-11
+800-53r5|AC-11(1)
+800-53r5|AC-12</t>
         </is>
       </c>
     </row>
@@ -12671,7 +14022,14 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>800-53|AC-2(5), 800-53|AC-11, 800-53|AC-11(1), 800-53|AC-12, 800-53r5|AC-2(5), 800-53r5|AC-11, 800-53r5|AC-11(1), 800-53r5|AC-12</t>
+          <t>800-53|AC-2(5)
+800-53|AC-11
+800-53|AC-11(1)
+800-53|AC-12
+800-53r5|AC-2(5)
+800-53r5|AC-11
+800-53r5|AC-11(1)
+800-53r5|AC-12</t>
         </is>
       </c>
     </row>
@@ -12715,7 +14073,16 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12759,7 +14126,16 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12798,7 +14174,16 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12836,7 +14221,8 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>800-53|AC-12, 800-53r5|AC-12</t>
+          <t>800-53|AC-12
+800-53r5|AC-12</t>
         </is>
       </c>
     </row>
@@ -12879,7 +14265,16 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12923,7 +14318,16 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>800-53|AC-17(2), 800-53|IA-5, 800-53|IA-5(1), 800-53|SC-8, 800-53|SC-8(1), 800-53r5|AC-17(2), 800-53r5|IA-5, 800-53r5|IA-5(1), 800-53r5|SC-8, 800-53r5|SC-8(1)</t>
+          <t>800-53|AC-17(2)
+800-53|IA-5
+800-53|IA-5(1)
+800-53|SC-8
+800-53|SC-8(1)
+800-53r5|AC-17(2)
+800-53r5|IA-5
+800-53r5|IA-5(1)
+800-53r5|SC-8
+800-53r5|SC-8(1)</t>
         </is>
       </c>
     </row>
@@ -12963,7 +14367,8 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>800-53|AC-2(12), 800-53r5|AC-2(12)</t>
+          <t>800-53|AC-2(12)
+800-53r5|AC-2(12)</t>
         </is>
       </c>
     </row>
@@ -13008,7 +14413,23 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>800-53|CM-2, 800-53|CM-6, 800-53|CM-7, 800-53|CM-7(1), 800-53|CM-9, 800-53|SA-3, 800-53|SA-8, 800-53|SA-10, 800-53r5|CM-1, 800-53r5|CM-2, 800-53r5|CM-6, 800-53r5|CM-7, 800-53r5|CM-7(1), 800-53r5|CM-9, 800-53r5|SA-3, 800-53r5|SA-8, 800-53r5|SA-10</t>
+          <t>800-53|CM-2
+800-53|CM-6
+800-53|CM-7
+800-53|CM-7(1)
+800-53|CM-9
+800-53|SA-3
+800-53|SA-8
+800-53|SA-10
+800-53r5|CM-1
+800-53r5|CM-2
+800-53r5|CM-6
+800-53r5|CM-7
+800-53r5|CM-7(1)
+800-53r5|CM-9
+800-53r5|SA-3
+800-53r5|SA-8
+800-53r5|SA-10</t>
         </is>
       </c>
     </row>
@@ -13045,7 +14466,10 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13082,7 +14506,10 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13120,7 +14547,10 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13158,7 +14588,10 @@
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13195,7 +14628,10 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13232,7 +14668,18 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13269,7 +14716,18 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13306,7 +14764,10 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13343,7 +14804,10 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13381,7 +14845,10 @@
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13419,7 +14886,10 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13456,7 +14926,10 @@
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13493,7 +14966,18 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13530,7 +15014,18 @@
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13567,7 +15062,10 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13604,7 +15102,10 @@
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13641,7 +15142,10 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13679,7 +15183,10 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13716,7 +15223,10 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13754,7 +15264,10 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13791,7 +15304,10 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>800-53|SC-7, 800-53|SC-7(5), 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|SC-7
+800-53|SC-7(5)
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13828,7 +15344,18 @@
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>
@@ -13865,7 +15392,18 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>800-53|AU-3, 800-53|AU-3(1), 800-53|AU-7, 800-53|AU-12, 800-53|SC-7, 800-53|SC-7(5), 800-53r5|AU-3, 800-53r5|AU-3(1), 800-53r5|AU-7, 800-53r5|AU-12, 800-53r5|SC-7, 800-53r5|SC-7(5)</t>
+          <t>800-53|AU-3
+800-53|AU-3(1)
+800-53|AU-7
+800-53|AU-12
+800-53|SC-7
+800-53|SC-7(5)
+800-53r5|AU-3
+800-53r5|AU-3(1)
+800-53r5|AU-7
+800-53r5|AU-12
+800-53r5|SC-7
+800-53r5|SC-7(5)</t>
         </is>
       </c>
     </row>

</xml_diff>